<commit_message>
Elementos para el Cableado.docx, consumo.xlsx
</commit_message>
<xml_diff>
--- a/consumo.xlsx
+++ b/consumo.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="18">
   <si>
     <t>Planta Baja</t>
   </si>
@@ -58,6 +58,18 @@
   </si>
   <si>
     <t>Expedición</t>
+  </si>
+  <si>
+    <t>Consumo total:</t>
+  </si>
+  <si>
+    <t>[W]</t>
+  </si>
+  <si>
+    <t>Resguardo:</t>
+  </si>
+  <si>
+    <t>C/Resguardo</t>
   </si>
 </sst>
 </file>
@@ -73,7 +85,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -86,8 +98,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -147,11 +165,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -162,6 +191,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -463,10 +497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:L40"/>
+  <dimension ref="B2:L41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -530,48 +564,56 @@
       <c r="C4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="7"/>
+      <c r="D4" s="7">
+        <v>1</v>
+      </c>
       <c r="E4" s="7">
         <v>100</v>
       </c>
       <c r="F4" s="7">
         <f>D4*E4</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="J4" s="7"/>
+      <c r="J4" s="7">
+        <v>2</v>
+      </c>
       <c r="K4" s="7">
         <v>100</v>
       </c>
       <c r="L4" s="7">
         <f>J4*K4</f>
-        <v>0</v>
+        <v>200</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="7"/>
+      <c r="D5" s="7">
+        <v>10</v>
+      </c>
       <c r="E5" s="7">
         <v>550</v>
       </c>
       <c r="F5" s="7">
         <f t="shared" ref="F5:F9" si="0">D5*E5</f>
-        <v>0</v>
+        <v>5500</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="J5" s="7"/>
+      <c r="J5" s="7">
+        <v>16</v>
+      </c>
       <c r="K5" s="7">
         <v>550</v>
       </c>
       <c r="L5" s="7">
         <f t="shared" ref="L5:L9" si="1">J5*K5</f>
-        <v>0</v>
+        <v>8800</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
@@ -589,33 +631,43 @@
       <c r="I6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J6" s="7"/>
+      <c r="J6" s="7">
+        <v>1</v>
+      </c>
       <c r="K6" s="7">
         <v>90</v>
       </c>
       <c r="L6" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
+      <c r="D7" s="7">
+        <v>1</v>
+      </c>
+      <c r="E7" s="7">
+        <v>30</v>
+      </c>
       <c r="F7" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="I7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
+      <c r="J7" s="7">
+        <v>2</v>
+      </c>
+      <c r="K7" s="7">
+        <v>30</v>
+      </c>
       <c r="L7" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
@@ -664,14 +716,30 @@
       </c>
       <c r="F10" s="7">
         <f>SUM(F4:F9)</f>
-        <v>0</v>
+        <v>5630</v>
       </c>
       <c r="K10" s="4" t="s">
         <v>12</v>
       </c>
       <c r="L10" s="7">
         <f>SUM(L4:L9)</f>
-        <v>0</v>
+        <v>9150</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="E11" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="9">
+        <f>F10+(F10*I33)</f>
+        <v>6756</v>
+      </c>
+      <c r="K11" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="L11" s="9">
+        <f>L10+(L10*$I$33)</f>
+        <v>10980</v>
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
@@ -726,48 +794,56 @@
       <c r="C14" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D14" s="7"/>
+      <c r="D14" s="7">
+        <v>2</v>
+      </c>
       <c r="E14" s="7">
         <v>100</v>
       </c>
       <c r="F14" s="7">
         <f>D14*E14</f>
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="J14" s="7"/>
+      <c r="J14" s="7">
+        <v>3</v>
+      </c>
       <c r="K14" s="7">
         <v>100</v>
       </c>
       <c r="L14" s="7">
         <f>J14*K14</f>
-        <v>0</v>
+        <v>300</v>
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C15" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D15" s="7"/>
+      <c r="D15" s="7">
+        <v>12</v>
+      </c>
       <c r="E15" s="7">
         <v>550</v>
       </c>
       <c r="F15" s="7">
         <f t="shared" ref="F15:F19" si="2">D15*E15</f>
-        <v>0</v>
+        <v>6600</v>
       </c>
       <c r="I15" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="J15" s="7"/>
+      <c r="J15" s="7">
+        <v>16</v>
+      </c>
       <c r="K15" s="7">
         <v>550</v>
       </c>
       <c r="L15" s="7">
         <f t="shared" ref="L15:L19" si="3">J15*K15</f>
-        <v>0</v>
+        <v>8800</v>
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
@@ -785,33 +861,43 @@
       <c r="I16" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J16" s="7"/>
+      <c r="J16" s="7">
+        <v>1</v>
+      </c>
       <c r="K16" s="7">
         <v>90</v>
       </c>
       <c r="L16" s="7">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C17" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
+      <c r="D17" s="7">
+        <v>1</v>
+      </c>
+      <c r="E17" s="7">
+        <v>30</v>
+      </c>
       <c r="F17" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="I17" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J17" s="7"/>
-      <c r="K17" s="7"/>
+      <c r="J17" s="7">
+        <v>2</v>
+      </c>
+      <c r="K17" s="7">
+        <v>30</v>
+      </c>
       <c r="L17" s="7">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.25">
@@ -860,14 +946,30 @@
       </c>
       <c r="F20" s="7">
         <f>SUM(F14:F19)</f>
-        <v>0</v>
+        <v>6830</v>
       </c>
       <c r="K20" s="4" t="s">
         <v>12</v>
       </c>
       <c r="L20" s="7">
         <f>SUM(L14:L19)</f>
-        <v>0</v>
+        <v>9250</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="E21" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F21" s="9">
+        <f>F20+(F20*$I$33)</f>
+        <v>8196</v>
+      </c>
+      <c r="K21" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="L21" s="9">
+        <f>L20+(L20*$I$33)</f>
+        <v>11100</v>
       </c>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.25">
@@ -922,48 +1024,56 @@
       <c r="C24" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D24" s="7"/>
+      <c r="D24" s="7">
+        <v>2</v>
+      </c>
       <c r="E24" s="7">
         <v>100</v>
       </c>
       <c r="F24" s="7">
         <f>D24*E24</f>
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="I24" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="J24" s="7"/>
+      <c r="J24" s="7">
+        <v>2</v>
+      </c>
       <c r="K24" s="7">
         <v>100</v>
       </c>
       <c r="L24" s="7">
         <f>J24*K24</f>
-        <v>0</v>
+        <v>200</v>
       </c>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C25" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D25" s="7"/>
+      <c r="D25" s="7">
+        <v>10</v>
+      </c>
       <c r="E25" s="7">
         <v>550</v>
       </c>
       <c r="F25" s="7">
         <f t="shared" ref="F25:F29" si="4">D25*E25</f>
-        <v>0</v>
+        <v>5500</v>
       </c>
       <c r="I25" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="J25" s="7"/>
+      <c r="J25" s="7">
+        <v>8</v>
+      </c>
       <c r="K25" s="7">
         <v>550</v>
       </c>
       <c r="L25" s="7">
         <f t="shared" ref="L25:L29" si="5">J25*K25</f>
-        <v>0</v>
+        <v>4400</v>
       </c>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.25">
@@ -994,20 +1104,28 @@
       <c r="C27" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
+      <c r="D27" s="7">
+        <v>1</v>
+      </c>
+      <c r="E27" s="7">
+        <v>30</v>
+      </c>
       <c r="F27" s="7">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="I27" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J27" s="7"/>
-      <c r="K27" s="7"/>
+      <c r="J27" s="7">
+        <v>1</v>
+      </c>
+      <c r="K27" s="7">
+        <v>30</v>
+      </c>
       <c r="L27" s="7">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.25">
@@ -1056,14 +1174,30 @@
       </c>
       <c r="F30" s="7">
         <f>SUM(F24:F29)</f>
-        <v>0</v>
+        <v>5730</v>
       </c>
       <c r="K30" s="4" t="s">
         <v>12</v>
       </c>
       <c r="L30" s="7">
         <f>SUM(L24:L29)</f>
-        <v>0</v>
+        <v>4630</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="E31" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F31" s="9">
+        <f>F30+(F30*$I$33)</f>
+        <v>6876</v>
+      </c>
+      <c r="K31" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="L31" s="9">
+        <f>L30+(L30*$I$33)</f>
+        <v>5556</v>
       </c>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.25">
@@ -1077,7 +1211,7 @@
       <c r="E32" s="2"/>
       <c r="F32" s="3"/>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B33" s="4" t="s">
         <v>2</v>
       </c>
@@ -1091,58 +1225,84 @@
       <c r="F33" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H33" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I33">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C34" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D34" s="7"/>
+      <c r="D34" s="7">
+        <v>1</v>
+      </c>
       <c r="E34" s="7">
         <v>100</v>
       </c>
       <c r="F34" s="7">
         <f>D34*E34</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+      <c r="H34" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I34">
+        <f>F11+L11+F21+L21+F31+L31+F41</f>
+        <v>51048</v>
+      </c>
+      <c r="J34" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C35" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D35" s="7"/>
+      <c r="D35" s="7">
+        <v>2</v>
+      </c>
       <c r="E35" s="7">
         <v>550</v>
       </c>
       <c r="F35" s="7">
         <f t="shared" ref="F35:F39" si="6">D35*E35</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C36" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D36" s="7"/>
+      <c r="D36" s="7">
+        <v>1</v>
+      </c>
       <c r="E36" s="7">
         <v>90</v>
       </c>
       <c r="F36" s="7">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C37" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D37" s="7"/>
-      <c r="E37" s="7"/>
+      <c r="D37" s="7">
+        <v>1</v>
+      </c>
+      <c r="E37" s="7">
+        <v>30</v>
+      </c>
       <c r="F37" s="7">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C38" s="4" t="s">
         <v>10</v>
       </c>
@@ -1153,7 +1313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C39" s="4" t="s">
         <v>11</v>
       </c>
@@ -1164,13 +1324,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E40" s="4" t="s">
         <v>12</v>
       </c>
       <c r="F40" s="7">
         <f>SUM(F34:F39)</f>
-        <v>0</v>
+        <v>1320</v>
+      </c>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="E41" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F41" s="9">
+        <f>F40+(F40*$I$33)</f>
+        <v>1584</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sabado por la tarde..
</commit_message>
<xml_diff>
--- a/consumo.xlsx
+++ b/consumo.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="32">
   <si>
     <t>Planta Baja</t>
   </si>
@@ -85,6 +85,33 @@
   </si>
   <si>
     <t>V</t>
+  </si>
+  <si>
+    <t>Planta Primer Subsuelo</t>
+  </si>
+  <si>
+    <t>Planta Segundo Subsuelo</t>
+  </si>
+  <si>
+    <t>Consumo</t>
+  </si>
+  <si>
+    <t>Subtotal</t>
+  </si>
+  <si>
+    <t>Camara IP Wi-Fi</t>
+  </si>
+  <si>
+    <t>Access Point</t>
+  </si>
+  <si>
+    <t>Servidor</t>
+  </si>
+  <si>
+    <t>Acces point</t>
+  </si>
+  <si>
+    <t>UPS</t>
   </si>
 </sst>
 </file>
@@ -126,7 +153,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -197,11 +224,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -224,7 +264,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -526,10 +596,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:M51"/>
+  <dimension ref="B2:M61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D119" sqref="D119"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -539,6 +609,7 @@
     <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.85546875" customWidth="1"/>
     <col min="13" max="13" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -608,14 +679,14 @@
         <v>4</v>
       </c>
       <c r="J4" s="7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K4" s="7">
         <v>100</v>
       </c>
       <c r="L4" s="7">
         <f>J4*K4</f>
-        <v>200</v>
+        <v>400</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
@@ -629,47 +700,49 @@
         <v>400</v>
       </c>
       <c r="F5" s="7">
-        <f t="shared" ref="F5:F9" si="0">D5*E5</f>
+        <f t="shared" ref="F5:F10" si="0">D5*E5</f>
         <v>4000</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>3</v>
       </c>
       <c r="J5" s="7">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K5" s="7">
         <v>400</v>
       </c>
       <c r="L5" s="7">
-        <f t="shared" ref="L5:L9" si="1">J5*K5</f>
-        <v>8000</v>
+        <f t="shared" ref="L5" si="1">J5*K5</f>
+        <v>8400</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="7"/>
+      <c r="D6" s="7">
+        <v>1</v>
+      </c>
       <c r="E6" s="7">
         <v>90</v>
       </c>
       <c r="F6" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J6" s="7">
         <v>1</v>
       </c>
       <c r="K6" s="7">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="L6" s="7">
-        <f t="shared" si="1"/>
-        <v>90</v>
+        <f>J6*K6</f>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
@@ -686,106 +759,106 @@
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="I7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="J7" s="7">
-        <v>2</v>
-      </c>
-      <c r="K7" s="7">
-        <v>30</v>
-      </c>
-      <c r="L7" s="7">
-        <f t="shared" si="1"/>
-        <v>60</v>
-      </c>
+      <c r="I7" s="4"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C8" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
+        <v>29</v>
+      </c>
+      <c r="D8" s="7">
+        <v>4</v>
+      </c>
+      <c r="E8" s="7">
+        <v>0</v>
+      </c>
       <c r="F8" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I8" s="4" t="s">
-        <v>10</v>
-      </c>
+      <c r="I8" s="4"/>
       <c r="J8" s="7"/>
       <c r="K8" s="7"/>
-      <c r="L8" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="L8" s="7"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
+        <v>30</v>
+      </c>
+      <c r="D9" s="7">
+        <v>1</v>
+      </c>
+      <c r="E9" s="7">
+        <v>4</v>
+      </c>
       <c r="F9" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
+        <v>4</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="L9" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>SUM(L4:L8)</f>
+        <v>8830</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E10" s="4" t="s">
+      <c r="C10" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="15">
+        <v>1</v>
+      </c>
+      <c r="E10" s="15">
+        <v>3000</v>
+      </c>
+      <c r="F10" s="15">
+        <f t="shared" si="0"/>
+        <v>3000</v>
+      </c>
+      <c r="K10" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="L10" s="15">
+        <f>L9+(L9*$I$40)</f>
+        <v>10596</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="E11" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="7">
-        <f>SUM(F4:F9)</f>
-        <v>4130</v>
-      </c>
-      <c r="K10" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="L10" s="7">
-        <f>SUM(L4:L9)</f>
-        <v>8350</v>
-      </c>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E11" s="14" t="s">
+      <c r="F11" s="28">
+        <f>SUM(F4:F10)</f>
+        <v>7224</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="L11" s="26">
+        <f>L10/$L$40</f>
+        <v>48.163636363636364</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="E12" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="F11" s="15">
-        <f>F10+(F10*I42)</f>
-        <v>4956</v>
-      </c>
-      <c r="K11" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="L11" s="15">
-        <f>L10+(L10*$I$42)</f>
-        <v>10020</v>
-      </c>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E12" s="4" t="s">
+      <c r="F12" s="15">
+        <f>F11+(F11*I40)</f>
+        <v>8668.7999999999993</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="E13" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F12" s="16">
-        <f>F11/$L$42</f>
-        <v>22.527272727272727</v>
-      </c>
-      <c r="K12" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="L12" s="16">
-        <f>L11/$L$42</f>
-        <v>45.545454545454547</v>
+      <c r="F13" s="26">
+        <f>F12/$L$40</f>
+        <v>39.403636363636359</v>
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
@@ -841,27 +914,27 @@
         <v>4</v>
       </c>
       <c r="D17" s="7">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E17" s="7">
         <v>100</v>
       </c>
       <c r="F17" s="7">
         <f>D17*E17</f>
-        <v>200</v>
+        <v>600</v>
       </c>
       <c r="I17" s="4" t="s">
         <v>4</v>
       </c>
       <c r="J17" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K17" s="7">
         <v>100</v>
       </c>
       <c r="L17" s="7">
         <f>J17*K17</f>
-        <v>300</v>
+        <v>200</v>
       </c>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.25">
@@ -869,581 +942,616 @@
         <v>3</v>
       </c>
       <c r="D18" s="7">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E18" s="7">
         <v>400</v>
       </c>
       <c r="F18" s="7">
-        <f t="shared" ref="F18:F22" si="2">D18*E18</f>
-        <v>4800</v>
+        <f t="shared" ref="F18" si="2">D18*E18</f>
+        <v>5600</v>
       </c>
       <c r="I18" s="4" t="s">
         <v>3</v>
       </c>
       <c r="J18" s="7">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="K18" s="7">
         <v>400</v>
       </c>
       <c r="L18" s="7">
-        <f t="shared" ref="L18:L22" si="3">J18*K18</f>
-        <v>6400</v>
+        <f t="shared" ref="L18" si="3">J18*K18</f>
+        <v>8400</v>
       </c>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C19" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D19" s="7"/>
+        <v>9</v>
+      </c>
+      <c r="D19" s="7">
+        <v>1</v>
+      </c>
       <c r="E19" s="7">
-        <v>90</v>
+        <v>35</v>
       </c>
       <c r="F19" s="7">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>D19*E19</f>
+        <v>35</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J19" s="7">
         <v>1</v>
       </c>
       <c r="K19" s="7">
-        <v>90</v>
+        <v>35</v>
       </c>
       <c r="L19" s="7">
-        <f t="shared" si="3"/>
-        <v>90</v>
+        <f>J19*K19</f>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C20" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D20" s="7">
-        <v>1</v>
-      </c>
-      <c r="E20" s="7">
-        <v>30</v>
-      </c>
-      <c r="F20" s="7">
-        <f t="shared" si="2"/>
-        <v>30</v>
-      </c>
-      <c r="I20" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="J20" s="7">
-        <v>2</v>
-      </c>
-      <c r="K20" s="7">
-        <v>30</v>
-      </c>
-      <c r="L20" s="7">
-        <f t="shared" si="3"/>
-        <v>60</v>
-      </c>
+      <c r="C20" s="4"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C21" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
+      <c r="E21" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="F21" s="7">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I21" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="J21" s="7"/>
-      <c r="K21" s="7"/>
+        <f>SUM(F17:F20)</f>
+        <v>6235</v>
+      </c>
+      <c r="K21" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="L21" s="7">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f>SUM(L17:L20)</f>
+        <v>8635</v>
       </c>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C22" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I22" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J22" s="7"/>
-      <c r="K22" s="7"/>
-      <c r="L22" s="7">
-        <f t="shared" si="3"/>
-        <v>0</v>
+      <c r="E22" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F22" s="15">
+        <f>F21+(F21*$I$40)</f>
+        <v>7482</v>
+      </c>
+      <c r="K22" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="L22" s="15">
+        <f>L21+(L21*$I$40)</f>
+        <v>10362</v>
       </c>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E23" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F23" s="7">
-        <f>SUM(F17:F22)</f>
-        <v>5030</v>
+        <v>20</v>
+      </c>
+      <c r="F23" s="26">
+        <f>F22/$L$40</f>
+        <v>34.009090909090908</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="L23" s="7">
-        <f>SUM(L17:L22)</f>
-        <v>6850</v>
-      </c>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E24" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="F24" s="15">
-        <f>F23+(F23*$I$42)</f>
-        <v>6036</v>
-      </c>
-      <c r="K24" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="L24" s="15">
-        <f>L23+(L23*$I$42)</f>
-        <v>8220</v>
-      </c>
-    </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E25" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F25" s="16">
-        <f>F24/$L$42</f>
-        <v>27.436363636363637</v>
-      </c>
-      <c r="K25" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="L25" s="16">
-        <f>L24/$L$42</f>
-        <v>37.363636363636367</v>
-      </c>
+      <c r="L23" s="26">
+        <f>L22/$L$40</f>
+        <v>47.1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B27" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" s="1">
+        <v>4</v>
+      </c>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="3"/>
+      <c r="H27" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I27" s="1">
+        <v>5</v>
+      </c>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="3"/>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B28" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C28" s="1">
-        <v>4</v>
-      </c>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="3"/>
+        <v>2</v>
+      </c>
+      <c r="C28" s="5"/>
+      <c r="D28" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="H28" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="I28" s="1">
+        <v>2</v>
+      </c>
+      <c r="I28" s="5"/>
+      <c r="J28" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="J28" s="2"/>
-      <c r="K28" s="2"/>
-      <c r="L28" s="3"/>
+      <c r="K28" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L28" s="4" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B29" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C29" s="5"/>
-      <c r="D29" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H29" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I29" s="5"/>
-      <c r="J29" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="K29" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="L29" s="4" t="s">
-        <v>7</v>
+      <c r="C29" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" s="7">
+        <v>4</v>
+      </c>
+      <c r="E29" s="7">
+        <v>100</v>
+      </c>
+      <c r="F29" s="7">
+        <f>D29*E29</f>
+        <v>400</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="J29" s="7">
+        <v>4</v>
+      </c>
+      <c r="K29" s="7">
+        <v>100</v>
+      </c>
+      <c r="L29" s="7">
+        <f>J29*K29</f>
+        <v>400</v>
       </c>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C30" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D30" s="7">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="E30" s="7">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="F30" s="7">
-        <f>D30*E30</f>
-        <v>200</v>
+        <f t="shared" ref="F30" si="4">D30*E30</f>
+        <v>3600</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J30" s="7">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="K30" s="7">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="L30" s="7">
-        <f>J30*K30</f>
-        <v>200</v>
+        <f t="shared" ref="L30" si="5">J30*K30</f>
+        <v>2800</v>
       </c>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C31" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D31" s="7">
+        <v>1</v>
+      </c>
+      <c r="E31" s="7">
+        <v>35</v>
+      </c>
+      <c r="F31" s="7">
+        <f>D31*E31</f>
+        <v>35</v>
+      </c>
+      <c r="I31" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J31" s="7">
+        <v>1</v>
+      </c>
+      <c r="K31" s="7">
+        <v>35</v>
+      </c>
+      <c r="L31" s="7">
+        <f>J31*K31</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C32" s="4"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+      <c r="I32" s="4"/>
+      <c r="J32" s="7"/>
+      <c r="K32" s="7"/>
+      <c r="L32" s="7"/>
+    </row>
+    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="E33" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F33" s="7">
+        <f>SUM(F29:F32)</f>
+        <v>4035</v>
+      </c>
+      <c r="K33" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="L33" s="7">
+        <f>SUM(L29:L32)</f>
+        <v>3235</v>
+      </c>
+    </row>
+    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="E34" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F34" s="15">
+        <f>F33+(F33*$I$40)</f>
+        <v>4842</v>
+      </c>
+      <c r="K34" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="L34" s="15">
+        <f>L33+(L33*$I$40)</f>
+        <v>3882</v>
+      </c>
+    </row>
+    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="E35" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F35" s="26">
+        <f>F34/$L$40</f>
+        <v>22.009090909090908</v>
+      </c>
+      <c r="K35" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="L35" s="26">
+        <f>L34/$L$40</f>
+        <v>17.645454545454545</v>
+      </c>
+    </row>
+    <row r="39" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B39" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="3"/>
+    </row>
+    <row r="40" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B40" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C40" s="5"/>
+      <c r="D40" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H40" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I40">
+        <v>0.2</v>
+      </c>
+      <c r="K40" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="L40">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C41" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D41" s="7">
+        <v>1</v>
+      </c>
+      <c r="E41" s="7">
+        <v>100</v>
+      </c>
+      <c r="F41" s="7">
+        <f>D41*E41</f>
+        <v>100</v>
+      </c>
+      <c r="H41" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I41">
+        <f>F12+L10+F22+L22+F34+L34+F47+F56+L56</f>
+        <v>47030.400000000009</v>
+      </c>
+      <c r="J41" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="42" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C42" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D31" s="7">
-        <v>10</v>
-      </c>
-      <c r="E31" s="7">
+      <c r="D42" s="7">
+        <v>2</v>
+      </c>
+      <c r="E42" s="7">
         <v>400</v>
       </c>
-      <c r="F31" s="7">
-        <f t="shared" ref="F31:F35" si="4">D31*E31</f>
-        <v>4000</v>
-      </c>
-      <c r="I31" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="J31" s="7">
-        <v>8</v>
-      </c>
-      <c r="K31" s="7">
-        <v>400</v>
-      </c>
-      <c r="L31" s="7">
-        <f t="shared" ref="L31:L35" si="5">J31*K31</f>
-        <v>3200</v>
-      </c>
-    </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C32" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7">
-        <v>90</v>
-      </c>
-      <c r="F32" s="7">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I32" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="J32" s="7"/>
-      <c r="K32" s="7">
-        <v>90</v>
-      </c>
-      <c r="L32" s="7">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="C33" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D33" s="7">
-        <v>1</v>
-      </c>
-      <c r="E33" s="7">
-        <v>30</v>
-      </c>
-      <c r="F33" s="7">
-        <f t="shared" si="4"/>
-        <v>30</v>
-      </c>
-      <c r="I33" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="J33" s="7">
-        <v>1</v>
-      </c>
-      <c r="K33" s="7">
-        <v>30</v>
-      </c>
-      <c r="L33" s="7">
-        <f t="shared" si="5"/>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="C34" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I34" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="J34" s="7"/>
-      <c r="K34" s="7"/>
-      <c r="L34" s="7">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="C35" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D35" s="7"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I35" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J35" s="7"/>
-      <c r="K35" s="7"/>
-      <c r="L35" s="7">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="E36" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F36" s="7">
-        <f>SUM(F30:F35)</f>
-        <v>4230</v>
-      </c>
-      <c r="K36" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="L36" s="7">
-        <f>SUM(L30:L35)</f>
-        <v>3430</v>
-      </c>
-    </row>
-    <row r="37" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="E37" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="F37" s="15">
-        <f>F36+(F36*$I$42)</f>
-        <v>5076</v>
-      </c>
-      <c r="K37" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="L37" s="15">
-        <f>L36+(L36*$I$42)</f>
-        <v>4116</v>
-      </c>
-    </row>
-    <row r="38" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="E38" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F38" s="16">
-        <f>F37/$L$42</f>
-        <v>23.072727272727274</v>
-      </c>
-      <c r="K38" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="L38" s="16">
-        <f>L37/$L$42</f>
-        <v>18.709090909090911</v>
-      </c>
-    </row>
-    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B41" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
-      <c r="F41" s="3"/>
-    </row>
-    <row r="42" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B42" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C42" s="5"/>
-      <c r="D42" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E42" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F42" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H42" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="I42">
-        <v>0.2</v>
-      </c>
-      <c r="K42" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="L42">
-        <v>220</v>
+      <c r="F42" s="7">
+        <f t="shared" ref="F42" si="6">D42*E42</f>
+        <v>800</v>
       </c>
     </row>
     <row r="43" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C43" s="4" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D43" s="7">
         <v>1</v>
       </c>
       <c r="E43" s="7">
-        <v>100</v>
+        <v>35</v>
       </c>
       <c r="F43" s="7">
         <f>D43*E43</f>
-        <v>100</v>
-      </c>
-      <c r="H43" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="I43">
-        <f>F11+L11+F24+L24+F37+L37+F50</f>
-        <v>39648</v>
-      </c>
-      <c r="J43" t="s">
-        <v>15</v>
+        <v>35</v>
+      </c>
+      <c r="H43" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="I43" s="12">
+        <f>I41/L40</f>
+        <v>213.77454545454549</v>
       </c>
     </row>
     <row r="44" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C44" s="4" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="D44" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E44" s="7">
-        <v>400</v>
+        <v>35</v>
       </c>
       <c r="F44" s="7">
-        <f t="shared" ref="F44:F48" si="6">D44*E44</f>
-        <v>800</v>
+        <f>D44*E44</f>
+        <v>35</v>
+      </c>
+      <c r="M44" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="45" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="C45" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D45" s="7">
-        <v>1</v>
-      </c>
-      <c r="E45" s="7">
-        <v>90</v>
-      </c>
-      <c r="F45" s="7">
-        <f t="shared" si="6"/>
-        <v>90</v>
-      </c>
-      <c r="H45" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="I45" s="12">
-        <f>I43/L42</f>
-        <v>180.21818181818182</v>
-      </c>
+      <c r="C45" s="4"/>
+      <c r="D45" s="7"/>
+      <c r="E45" s="7"/>
+      <c r="F45" s="7"/>
     </row>
     <row r="46" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="C46" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D46" s="7">
-        <v>1</v>
-      </c>
-      <c r="E46" s="7">
-        <v>30</v>
+      <c r="E46" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="F46" s="7">
-        <f t="shared" si="6"/>
-        <v>30</v>
-      </c>
-      <c r="M46" t="s">
-        <v>19</v>
+        <f>SUM(F41:F45)</f>
+        <v>970</v>
       </c>
     </row>
     <row r="47" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="C47" s="4" t="s">
+      <c r="E47" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F47" s="15">
+        <f>F46+(F46*$I$40)</f>
+        <v>1164</v>
+      </c>
+    </row>
+    <row r="48" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="E48" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F48" s="26">
+        <f>F47/$L$40</f>
+        <v>5.290909090909091</v>
+      </c>
+    </row>
+    <row r="51" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B51" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D51" s="3"/>
+      <c r="H51" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J51" s="3"/>
+    </row>
+    <row r="52" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B52" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C52" s="4"/>
+      <c r="D52" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="E52" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="F52" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="H52" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="I52" s="5"/>
+      <c r="J52" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="K52" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="L52" s="16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="53" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C53" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D53" s="7">
+        <v>2</v>
+      </c>
+      <c r="E53" s="18">
+        <v>5</v>
+      </c>
+      <c r="F53" s="18">
+        <f>E53*D53</f>
         <v>10</v>
       </c>
-      <c r="D47" s="7"/>
-      <c r="E47" s="7"/>
-      <c r="F47" s="7">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="C48" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D48" s="7"/>
-      <c r="E48" s="7"/>
-      <c r="F48" s="7">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E49" s="4" t="s">
+      <c r="I53" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="J53" s="7">
+        <v>2</v>
+      </c>
+      <c r="K53" s="18">
+        <v>5</v>
+      </c>
+      <c r="L53" s="18">
+        <f>K53*J53</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="54" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C54" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D54" s="18">
+        <v>1</v>
+      </c>
+      <c r="E54" s="18">
+        <v>4</v>
+      </c>
+      <c r="F54" s="18">
+        <f>E54*D54</f>
+        <v>4</v>
+      </c>
+      <c r="I54" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J54" s="18">
+        <v>1</v>
+      </c>
+      <c r="K54" s="18">
+        <v>4</v>
+      </c>
+      <c r="L54" s="18">
+        <f>K54*J54</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B55" s="19"/>
+      <c r="C55" s="23"/>
+      <c r="D55" s="20"/>
+      <c r="E55" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F49" s="7">
-        <f>SUM(F43:F48)</f>
-        <v>1020</v>
-      </c>
-    </row>
-    <row r="50" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E50" s="14" t="s">
+      <c r="F55" s="18">
+        <f>SUM(F53:F54)</f>
+        <v>14</v>
+      </c>
+      <c r="I55" s="23"/>
+      <c r="J55" s="24"/>
+      <c r="K55" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="L55" s="18">
+        <f>SUM(L53:L54)</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="56" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B56" s="19"/>
+      <c r="C56" s="23"/>
+      <c r="D56" s="21"/>
+      <c r="E56" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="F50" s="15">
-        <f>F49+(F49*$I$42)</f>
-        <v>1224</v>
-      </c>
-    </row>
-    <row r="51" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E51" s="4" t="s">
+      <c r="F56" s="18">
+        <f>F55+F55*I40</f>
+        <v>16.8</v>
+      </c>
+      <c r="I56" s="23"/>
+      <c r="J56" s="25"/>
+      <c r="K56" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="L56" s="18">
+        <f>L55+L55*I40</f>
+        <v>16.8</v>
+      </c>
+    </row>
+    <row r="57" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="E57" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F51" s="16">
-        <f>F50/$L$42</f>
-        <v>5.5636363636363635</v>
-      </c>
+      <c r="F57" s="26">
+        <f>F56/L40</f>
+        <v>7.636363636363637E-2</v>
+      </c>
+      <c r="K57" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="L57" s="26">
+        <f>L56/L40</f>
+        <v>7.636363636363637E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D61" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1455,7 +1563,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>

</xml_diff>